<commit_message>
added remaining u-net layers to follow Ronneberger2015, also added dropout layers in what i think are the correct locations... added one-hot encoding for segmentation masks (with decoding in mask overlay generation function); updated u-net dimension spreadsheet.
</commit_message>
<xml_diff>
--- a/u-net-dimensions.xlsx
+++ b/u-net-dimensions.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f002r5k\GitHub\ralpn-seg\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E55EDD-E0FA-4FDA-8642-FD6FF4B45620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="7656"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="8">
   <si>
     <t>x2</t>
   </si>
@@ -46,11 +55,14 @@
   <si>
     <t>change to zero to get padding -&gt;</t>
   </si>
+  <si>
+    <t>CROP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -239,15 +251,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -262,6 +265,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -544,44 +556,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="22" width="8.88671875" style="19"/>
+    <col min="11" max="22" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-    </row>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="13"/>
+    </row>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -597,24 +611,24 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="22" t="s">
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
       <c r="X2" t="s">
         <v>2</v>
       </c>
@@ -625,7 +639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
         <f>D5*D3+C3</f>
         <v>512</v>
@@ -642,26 +656,29 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
       <c r="R3" s="9">
         <f>(P5-Q5)*R5</f>
         <v>324</v>
       </c>
-      <c r="S3" s="17">
-        <v>4</v>
-      </c>
-      <c r="T3" s="23">
+      <c r="S3" s="14">
+        <v>4</v>
+      </c>
+      <c r="T3" s="20">
         <f>R3-S3</f>
         <v>320</v>
       </c>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
+      <c r="U3" s="14">
+        <f>(D5*D3-R3)/2</f>
+        <v>92</v>
+      </c>
+      <c r="V3" s="14"/>
       <c r="X3" s="2">
         <f>Z5*Z3+Y3</f>
         <v>512</v>
@@ -673,7 +690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <f>B3-512</f>
         <v>0</v>
@@ -692,27 +709,27 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="S4" s="17"/>
-      <c r="T4" s="24">
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="14"/>
+      <c r="T4" s="21">
         <f>T3-512</f>
         <v>-192</v>
       </c>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
       <c r="Z4" t="s">
         <v>2</v>
       </c>
@@ -723,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="7"/>
       <c r="D5" s="9">
@@ -740,25 +757,28 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="9">
         <f>(N7-O7)*P7</f>
         <v>168</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="Q5" s="14">
         <v>6</v>
       </c>
-      <c r="R5" s="17">
-        <v>2</v>
-      </c>
-      <c r="S5" s="17"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
+      <c r="R5" s="14">
+        <v>2</v>
+      </c>
+      <c r="S5" s="14"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="14">
+        <f>(F7*F5-P5)/2</f>
+        <v>40</v>
+      </c>
+      <c r="V5" s="14"/>
       <c r="Z5" s="1">
         <f>AB7*AB5+AA5</f>
         <v>254</v>
@@ -770,7 +790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -786,24 +806,24 @@
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
       <c r="AB6" t="s">
         <v>2</v>
       </c>
@@ -814,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -831,25 +851,28 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
       <c r="N7" s="9">
         <f>(L9-M9)*N9</f>
         <v>88</v>
       </c>
-      <c r="O7" s="17">
-        <v>4</v>
-      </c>
-      <c r="P7" s="17">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
+      <c r="O7" s="14">
+        <v>4</v>
+      </c>
+      <c r="P7" s="14">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="14">
+        <f>(H9*H7-N7)/2</f>
+        <v>16</v>
+      </c>
+      <c r="V7" s="14"/>
       <c r="AB7" s="1">
         <f>AD9*AD7+AC7</f>
         <v>126</v>
@@ -861,7 +884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -877,24 +900,24 @@
       <c r="J8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
       <c r="AD8" t="s">
         <v>2</v>
       </c>
@@ -905,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -922,25 +945,28 @@
       <c r="J9" s="7">
         <v>2</v>
       </c>
-      <c r="K9" s="17"/>
+      <c r="K9" s="14"/>
       <c r="L9" s="9">
         <f>(J11-K11)*L11</f>
         <v>48</v>
       </c>
-      <c r="M9" s="17">
-        <v>4</v>
-      </c>
-      <c r="N9" s="17">
-        <v>2</v>
-      </c>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
+      <c r="M9" s="14">
+        <v>4</v>
+      </c>
+      <c r="N9" s="14">
+        <v>2</v>
+      </c>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="14">
+        <f>(J11*J9-L9)/2</f>
+        <v>4</v>
+      </c>
+      <c r="V9" s="14"/>
       <c r="AD9" s="1">
         <f>AF11*AF9+AE9</f>
         <v>62</v>
@@ -952,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -964,27 +990,27 @@
       <c r="J10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
+      <c r="K10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
       <c r="AF10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -995,56 +1021,58 @@
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
-      <c r="J11" s="27">
+      <c r="J11" s="24">
         <v>28</v>
       </c>
-      <c r="K11" s="25">
-        <v>4</v>
-      </c>
-      <c r="L11" s="25">
-        <v>2</v>
-      </c>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
+      <c r="K11" s="22">
+        <v>4</v>
+      </c>
+      <c r="L11" s="22">
+        <v>2</v>
+      </c>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
       <c r="AF11" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="13" t="s">
+    <row r="12" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-    </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V13" s="13"/>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
@@ -1060,26 +1088,26 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="S14" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="T14" s="22" t="s">
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="S14" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="T14" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-    </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <f>D17*D15+C15</f>
         <v>572</v>
@@ -1096,28 +1124,31 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
       <c r="R15" s="9">
         <f>(P17-Q17)*R17</f>
         <v>392</v>
       </c>
-      <c r="S15" s="17">
-        <v>4</v>
-      </c>
-      <c r="T15" s="23">
+      <c r="S15" s="14">
+        <v>4</v>
+      </c>
+      <c r="T15" s="20">
         <f>R15-S15</f>
         <v>388</v>
       </c>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
-    </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="U15" s="14">
+        <f>(D17*D15-R15)/2</f>
+        <v>88</v>
+      </c>
+      <c r="V15" s="14"/>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
         <f>B15-512</f>
         <v>60</v>
@@ -1136,29 +1167,29 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="S16" s="17"/>
-      <c r="T16" s="24">
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" s="14"/>
+      <c r="T16" s="21">
         <f>T15-512</f>
         <v>-124</v>
       </c>
-      <c r="U16" s="17"/>
-      <c r="V16" s="17"/>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" s="7"/>
       <c r="D17" s="9">
@@ -1175,27 +1206,30 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
       <c r="P17" s="9">
         <f>(N19-O19)*P19</f>
         <v>200</v>
       </c>
-      <c r="Q17" s="17">
-        <v>4</v>
-      </c>
-      <c r="R17" s="17">
-        <v>2</v>
-      </c>
-      <c r="S17" s="17"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="Q17" s="14">
+        <v>4</v>
+      </c>
+      <c r="R17" s="14">
+        <v>2</v>
+      </c>
+      <c r="S17" s="14"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="14">
+        <f>(F19*F17-P17)/2</f>
+        <v>40</v>
+      </c>
+      <c r="V17" s="14"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1211,26 +1245,26 @@
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="O18" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="P18" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="17"/>
-      <c r="V18" s="17"/>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1247,27 +1281,30 @@
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
       <c r="N19" s="9">
         <f>(L21-M21)*N21</f>
         <v>104</v>
       </c>
-      <c r="O19" s="17">
-        <v>4</v>
-      </c>
-      <c r="P19" s="17">
-        <v>2</v>
-      </c>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="17"/>
-      <c r="V19" s="17"/>
-    </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="O19" s="14">
+        <v>4</v>
+      </c>
+      <c r="P19" s="14">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="14">
+        <f>(H21*H19-N19)/2</f>
+        <v>16</v>
+      </c>
+      <c r="V19" s="14"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1283,26 +1320,26 @@
       <c r="J20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M20" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="17"/>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K20" s="14"/>
+      <c r="L20" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1319,27 +1356,30 @@
       <c r="J21" s="7">
         <v>2</v>
       </c>
-      <c r="K21" s="17"/>
+      <c r="K21" s="14"/>
       <c r="L21" s="9">
         <f>(J23-K23)*L23</f>
         <v>56</v>
       </c>
-      <c r="M21" s="17">
-        <v>4</v>
-      </c>
-      <c r="N21" s="17">
-        <v>2</v>
-      </c>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="17"/>
-      <c r="V21" s="17"/>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="M21" s="14">
+        <v>4</v>
+      </c>
+      <c r="N21" s="14">
+        <v>2</v>
+      </c>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="14">
+        <f>(J23*J21-L21)/2</f>
+        <v>4</v>
+      </c>
+      <c r="V21" s="14"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1351,24 +1391,24 @@
       <c r="J22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L22" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="17"/>
-      <c r="V22" s="17"/>
-    </row>
-    <row r="23" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K22" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="14"/>
+    </row>
+    <row r="23" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -1379,25 +1419,25 @@
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
-      <c r="J23" s="27">
+      <c r="J23" s="24">
         <v>32</v>
       </c>
-      <c r="K23" s="25">
-        <v>4</v>
-      </c>
-      <c r="L23" s="25">
-        <v>2</v>
-      </c>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="20"/>
-      <c r="V23" s="20"/>
+      <c r="K23" s="22">
+        <v>4</v>
+      </c>
+      <c r="L23" s="22">
+        <v>2</v>
+      </c>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
changed u-net dimensions to volumetric
</commit_message>
<xml_diff>
--- a/u-net-dimensions.xlsx
+++ b/u-net-dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f002r5k\GitHub\ralpn-seg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E55EDD-E0FA-4FDA-8642-FD6FF4B45620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467654BB-7FC9-43C6-B55C-A7803FE61990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
   <dimension ref="B1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
     <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
         <f>D5*D3+C3</f>
-        <v>512</v>
+        <v>704</v>
       </c>
       <c r="C3" s="7">
         <v>4</v>
@@ -665,14 +665,14 @@
       <c r="Q3" s="14"/>
       <c r="R3" s="9">
         <f>(P5-Q5)*R5</f>
-        <v>324</v>
+        <v>516</v>
       </c>
       <c r="S3" s="14">
         <v>4</v>
       </c>
       <c r="T3" s="20">
         <f>R3-S3</f>
-        <v>320</v>
+        <v>512</v>
       </c>
       <c r="U3" s="14">
         <f>(D5*D3-R3)/2</f>
@@ -693,7 +693,7 @@
     <row r="4" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <f>B3-512</f>
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
@@ -726,7 +726,7 @@
       <c r="S4" s="14"/>
       <c r="T4" s="21">
         <f>T3-512</f>
-        <v>-192</v>
+        <v>0</v>
       </c>
       <c r="U4" s="14"/>
       <c r="V4" s="14"/>
@@ -745,7 +745,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="9">
         <f>F7*F5+E5</f>
-        <v>254</v>
+        <v>350</v>
       </c>
       <c r="E5" s="10">
         <v>6</v>
@@ -764,7 +764,7 @@
       <c r="O5" s="14"/>
       <c r="P5" s="9">
         <f>(N7-O7)*P7</f>
-        <v>168</v>
+        <v>264</v>
       </c>
       <c r="Q5" s="14">
         <v>6</v>
@@ -841,7 +841,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="9">
         <f>H9*H7+G7</f>
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="G7" s="7">
         <v>4</v>
@@ -856,7 +856,7 @@
       <c r="M7" s="14"/>
       <c r="N7" s="9">
         <f>(L9-M9)*N9</f>
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="O7" s="14">
         <v>4</v>
@@ -937,7 +937,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="9">
         <f>J11*J9+I9</f>
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="I9" s="7">
         <v>4</v>
@@ -948,7 +948,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="9">
         <f>(J11-K11)*L11</f>
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="M9" s="14">
         <v>4</v>
@@ -1022,7 +1022,7 @@
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
       <c r="J11" s="24">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="K11" s="22">
         <v>4</v>

</xml_diff>